<commit_message>
added framework_variant to settings worksheet
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework.clean/framework.xlsx
+++ b/app/config/assets/framework/forms/framework.clean/framework.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clarice\odk-reference\app-designer\app\config\assets\framework\forms\framework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tvpri\my_projects\edu\au\tpricew\app-designer\app\config\assets\framework\forms\framework.clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4FF0AA8-2A1C-42A2-9EB6-F8C2CB1668A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="5"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="240">
   <si>
     <t>comments</t>
   </si>
@@ -770,11 +771,17 @@
   <si>
     <t>text.en</t>
   </si>
+  <si>
+    <t>framework_variant</t>
+  </si>
+  <si>
+    <t>clean</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -917,11 +924,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -934,13 +941,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1051,9 +1052,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1091,7 +1092,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1163,7 +1164,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1336,20 +1337,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1357,7 +1358,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>15</v>
       </c>
@@ -1373,25 +1374,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="101.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="46.140625" customWidth="1"/>
+    <col min="2" max="2" width="101.109375" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="4" max="4" width="46.109375" customWidth="1"/>
     <col min="5" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="8" max="8" width="31.42578125" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.88671875" customWidth="1"/>
+    <col min="8" max="8" width="31.44140625" customWidth="1"/>
+    <col min="9" max="9" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -1418,7 +1419,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>17</v>
       </c>
@@ -1427,7 +1428,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
         <v>21</v>
       </c>
@@ -1438,13 +1439,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>19</v>
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>2</v>
       </c>
@@ -1455,23 +1456,23 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>156</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="3" t="s">
         <v>158</v>
@@ -1483,7 +1484,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
@@ -1502,21 +1503,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1527,7 +1528,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -1550,20 +1551,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="8" width="24.7109375" customWidth="1"/>
-    <col min="9" max="9" width="41.140625" customWidth="1"/>
+    <col min="3" max="8" width="24.6640625" customWidth="1"/>
+    <col min="9" max="9" width="41.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1595,7 +1596,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
@@ -1609,7 +1610,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1626,7 +1627,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1637,7 +1638,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1657,8 +1658,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>238</v>
+      </c>
+      <c r="B6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>161</v>
       </c>
@@ -1672,7 +1680,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>162</v>
       </c>
@@ -1686,7 +1694,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>171</v>
       </c>
@@ -1700,7 +1708,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1710,13 +1718,13 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
     </row>
-    <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
     </row>
-    <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1726,7 +1734,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1736,13 +1744,13 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
     </row>
-    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1752,7 +1760,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1762,10 +1770,10 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
     </row>
-    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
     </row>
   </sheetData>
@@ -1775,686 +1783,685 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="57.85546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="56.140625" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="57.88671875" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" customWidth="1"/>
+    <col min="4" max="4" width="56.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" t="s">
         <v>165</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" t="s">
         <v>148</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" t="s">
         <v>150</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:4" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>129</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:4" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" t="s">
         <v>79</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>80</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" t="s">
         <v>81</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>82</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>84</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>86</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" t="s">
         <v>87</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>88</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" t="s">
         <v>89</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" t="s">
         <v>94</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
+    <row r="28" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>109</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="5" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
+    <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>98</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" t="s">
         <v>96</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="5" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>99</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" t="s">
         <v>100</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
+    <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" t="s">
         <v>102</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>103</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" t="s">
         <v>106</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>104</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="6" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>107</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" t="s">
         <v>108</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="178.5" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
+    <row r="36" spans="1:4" ht="184.8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>110</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="5" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
+    <row r="37" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>112</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" t="s">
         <v>113</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A38" s="6" t="s">
+    <row r="38" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>116</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" t="s">
         <v>114</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D38" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A39" s="6" t="s">
+    <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" t="s">
         <v>117</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A40" s="6" t="s">
+    <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>118</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" t="s">
         <v>119</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="5" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A41" s="6" t="s">
+    <row r="41" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>120</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" t="s">
         <v>121</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D41" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="6" t="s">
+    <row r="42" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>122</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" t="s">
         <v>123</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A43" s="6" t="s">
+    <row r="43" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>124</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" t="s">
         <v>125</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="6" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>126</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" t="s">
         <v>127</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="5" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="6" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>128</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" t="s">
         <v>39</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" t="s">
         <v>40</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D45" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="6" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>130</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" t="s">
         <v>146</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D46" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A47" s="6" t="s">
+    <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>131</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" t="s">
         <v>132</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D47" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A48" s="6" t="s">
+    <row r="48" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>133</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" t="s">
         <v>134</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D48" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A49" s="6" t="s">
+    <row r="49" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>135</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" t="s">
         <v>136</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="5" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="6" t="s">
+    <row r="50" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>137</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" t="s">
         <v>138</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="5" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A51" s="6" t="s">
+    <row r="51" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>141</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" t="s">
         <v>139</v>
       </c>
-      <c r="D51" s="6" t="s">
+      <c r="D51" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A52" s="6" t="s">
+    <row r="52" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>142</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" t="s">
         <v>102</v>
       </c>
-      <c r="D52" s="6" t="s">
+      <c r="D52" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A53" s="6" t="s">
+    <row r="53" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>143</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" t="s">
         <v>140</v>
       </c>
-      <c r="D53" s="6" t="s">
+      <c r="D53" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A54" s="6" t="s">
+    <row r="54" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>144</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" t="s">
         <v>132</v>
       </c>
-      <c r="D54" s="6" t="s">
+      <c r="D54" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="6" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>145</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" t="s">
         <v>147</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="D55" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="6" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>151</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" t="s">
         <v>152</v>
       </c>
-      <c r="D56" s="6" t="s">
+      <c r="D56" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="6" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>154</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" t="s">
         <v>153</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="D57" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="7" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="D58" s="6" t="s">
+      <c r="D58" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="7" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="D59" s="6" t="s">
+      <c r="D59" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="7" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B60" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D60" s="6" t="s">
+      <c r="D60" t="s">
         <v>176</v>
       </c>
     </row>
@@ -2465,23 +2472,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
+    <col min="5" max="5" width="28.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
added framework_variant to framework and framework.clean
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework.clean/framework.xlsx
+++ b/app/config/assets/framework/forms/framework.clean/framework.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clarice\odk-reference\app-designer\app\config\assets\framework\forms\framework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tvpri\my_projects\edu\au\tpricew\app-designer\app\config\assets\framework\forms\framework.clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF54393-2766-47CD-9988-144903BF23D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="240">
   <si>
     <t>comments</t>
   </si>
@@ -770,11 +771,17 @@
   <si>
     <t>text.en</t>
   </si>
+  <si>
+    <t>clean</t>
+  </si>
+  <si>
+    <t>framework_variant</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -917,11 +924,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -934,13 +941,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1051,9 +1052,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1091,7 +1092,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1163,7 +1164,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1336,20 +1337,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1357,7 +1358,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>15</v>
       </c>
@@ -1373,25 +1374,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="101.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="46.140625" customWidth="1"/>
+    <col min="2" max="2" width="101.109375" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="4" max="4" width="46.109375" customWidth="1"/>
     <col min="5" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="8" max="8" width="31.42578125" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.88671875" customWidth="1"/>
+    <col min="8" max="8" width="31.44140625" customWidth="1"/>
+    <col min="9" max="9" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -1418,7 +1419,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>17</v>
       </c>
@@ -1427,7 +1428,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
         <v>21</v>
       </c>
@@ -1438,13 +1439,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>19</v>
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>2</v>
       </c>
@@ -1455,23 +1456,23 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>156</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="3" t="s">
         <v>158</v>
@@ -1483,7 +1484,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
@@ -1502,21 +1503,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1527,7 +1528,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -1550,20 +1551,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="8" width="24.7109375" customWidth="1"/>
-    <col min="9" max="9" width="41.140625" customWidth="1"/>
+    <col min="3" max="8" width="24.6640625" customWidth="1"/>
+    <col min="9" max="9" width="41.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1595,7 +1596,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
@@ -1609,7 +1610,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1626,7 +1627,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1637,7 +1638,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1657,8 +1658,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>239</v>
+      </c>
+      <c r="B6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>161</v>
       </c>
@@ -1672,7 +1680,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>162</v>
       </c>
@@ -1686,7 +1694,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>171</v>
       </c>
@@ -1700,7 +1708,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1710,13 +1718,13 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
     </row>
-    <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
     </row>
-    <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1726,7 +1734,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1736,13 +1744,13 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
     </row>
-    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1752,7 +1760,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1762,10 +1770,10 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
     </row>
-    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
     </row>
   </sheetData>
@@ -1775,686 +1783,685 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="57.85546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="56.140625" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="57.88671875" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" customWidth="1"/>
+    <col min="4" max="4" width="56.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" t="s">
         <v>165</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" t="s">
         <v>148</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" t="s">
         <v>150</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:4" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>129</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:4" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" t="s">
         <v>79</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>80</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" t="s">
         <v>81</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>82</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>84</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>86</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" t="s">
         <v>87</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>88</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" t="s">
         <v>89</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" t="s">
         <v>94</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
+    <row r="28" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>109</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="5" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
+    <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>98</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" t="s">
         <v>96</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="5" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>99</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" t="s">
         <v>100</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
+    <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" t="s">
         <v>102</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>103</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" t="s">
         <v>106</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>104</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="6" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>107</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" t="s">
         <v>108</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="178.5" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
+    <row r="36" spans="1:4" ht="184.8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>110</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="5" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
+    <row r="37" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>112</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" t="s">
         <v>113</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A38" s="6" t="s">
+    <row r="38" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>116</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" t="s">
         <v>114</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D38" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A39" s="6" t="s">
+    <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" t="s">
         <v>117</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A40" s="6" t="s">
+    <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>118</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" t="s">
         <v>119</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="5" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A41" s="6" t="s">
+    <row r="41" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>120</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" t="s">
         <v>121</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D41" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="6" t="s">
+    <row r="42" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>122</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" t="s">
         <v>123</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A43" s="6" t="s">
+    <row r="43" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>124</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" t="s">
         <v>125</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="6" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>126</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" t="s">
         <v>127</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="5" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="6" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>128</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" t="s">
         <v>39</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" t="s">
         <v>40</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D45" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="6" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>130</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" t="s">
         <v>146</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D46" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A47" s="6" t="s">
+    <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>131</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" t="s">
         <v>132</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D47" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A48" s="6" t="s">
+    <row r="48" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>133</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" t="s">
         <v>134</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D48" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A49" s="6" t="s">
+    <row r="49" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>135</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" t="s">
         <v>136</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="5" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="6" t="s">
+    <row r="50" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>137</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" t="s">
         <v>138</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="5" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A51" s="6" t="s">
+    <row r="51" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>141</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" t="s">
         <v>139</v>
       </c>
-      <c r="D51" s="6" t="s">
+      <c r="D51" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A52" s="6" t="s">
+    <row r="52" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>142</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" t="s">
         <v>102</v>
       </c>
-      <c r="D52" s="6" t="s">
+      <c r="D52" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A53" s="6" t="s">
+    <row r="53" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>143</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" t="s">
         <v>140</v>
       </c>
-      <c r="D53" s="6" t="s">
+      <c r="D53" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A54" s="6" t="s">
+    <row r="54" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>144</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" t="s">
         <v>132</v>
       </c>
-      <c r="D54" s="6" t="s">
+      <c r="D54" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="6" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>145</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" t="s">
         <v>147</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="D55" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="6" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>151</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" t="s">
         <v>152</v>
       </c>
-      <c r="D56" s="6" t="s">
+      <c r="D56" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="6" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>154</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" t="s">
         <v>153</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="D57" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="7" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="D58" s="6" t="s">
+      <c r="D58" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="7" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="D59" s="6" t="s">
+      <c r="D59" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="7" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B60" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D60" s="6" t="s">
+      <c r="D60" t="s">
         <v>176</v>
       </c>
     </row>
@@ -2465,23 +2472,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
+    <col min="5" max="5" width="28.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>35</v>
       </c>

</xml_diff>